<commit_message>
working code added reply to
</commit_message>
<xml_diff>
--- a/TodayRequriments.xlsx
+++ b/TodayRequriments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2360,6 +2360,1069 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>"Isaac, Centraprise" &lt;isaac@centraprise.com&gt;</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>469-923-8111</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Java Developer at NYC NY (Day One Onsite) Need Ex Cognizant OR Ex Amex</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>"Mehak Pandey, Simplify Software Experts" &lt;mehak@simplifysoftwareexperts.com&gt;</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>(201)2855932</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>CORE JAVA BACKEND DEVELOPER</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>"Raman Arora, Zealhire" &lt;raman@zealhire.com&gt;</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>(332) 2878468</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>IT Oracle Project Managers :: hybrid role :: Local Only</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Vishwas Vishwas &lt;vishwasvishwas622@gmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>55867-92544</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Sr Golang Developers || Rosemont, IL/Onsite)</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>amit &lt;amitcorp2corp@gmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>848-666-1490</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Opening for Oracle Supplier Data Hub (Oracle SDH)</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>amit &lt;amitcorp2corp@gmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>848-666-1490</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>{C2C-W2 -Jobs} Opening for Oracle Supplier Data Hub (Oracle SDH)</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Pankaj Chauhan &lt;pchauhan@accroid.com&gt;</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>(302)-4851559</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Oracle EBS IT Project Manager || Minneapolis, MN (On-Site) relocation
+ works  || Visa: USC/GC</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>ajay.sai@dprsolutionsinc.com</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>5714632218, (603) 4860938</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Resume Submission Java Full Stack Developer</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Vineeth Damarla &lt;ron@americanitsystems.com&gt;</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>125.36132370</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Java Technical Developer | Berkeley Heights, NJ 100% onsite from
+ day-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Vineeth Damarla &lt;ron@americanitsystems.com&gt;</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>125.36132370</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Java Technical Developer | Berkeley Heights, NJ (100% onsite from
+ day-1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>"Shivam Tayal, Quantum World Technologies Inc" &lt;shivam.tayal@quantumworldit.com&gt;</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>+1 805-6784659</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Hiring Oracle Sales Cloud SDH Consultant, Chicago IL</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>"sachin, Atlas Cloud, solution" &lt;sachin@acloudinc.com&gt;</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>+1 4195959070</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Microsoft Dynamics D365</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>"Vignesh Ramakrishnan, Teamware solution" &lt;vignesh.r@twsol.com&gt;</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>+12145449254</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Need-Oracle Supplier Data Hub consultant Chicago, IL</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Jaffer Shahul H &lt;shahul.h@diamondpick.com&gt;</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>34843418293, 6042538933</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Immediate Hire - Microsoft SQL Server (DBA - Architect/ Consultant) -
+ Reading, PA(Hybrid) - Only Local</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>"irfan shiak, Agile Enterprise Solutions Inc." &lt;irfan_shaik@aesincus.com&gt;</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>647-375-2228, 972-440-0069</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>SingleStore DBA with Python Programming |Austin, TX| Onsite</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>"Suzanne Rogers, Concord IT Systems" &lt;suzanne.rogers@concorditsystems.com&gt;</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>17866280721</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Immediate hiring for Oracle NetSuite Functional Consultant - Remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>"Satish Kumar, Donato Technologies INC" &lt;satish@donatotech.net&gt;</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>(469) 9299409, 469-533-0333</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Looking for JPC - 2122 - Oracle IAM Architect -Latham, New York (Onsite)- Contract Job- Sligo</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Surya Hemanth &lt;hemanth@brillius.com&gt;</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>+1 510-4008680</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>JAVA DEVELOPER WITH ML Exp :: Bellevue, WA</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>"Suraj Prashar, Pivotal Technologies" &lt;suraj.prashar@pivotal-technologies.com&gt;</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>(703) 5708775</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Urgent Requirement || SQL DBA || Remote|| 6+Months</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>"Pallavi, Yochana" &lt;pallavi@yochana.com&gt;</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>2482373189</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Please share local candidates-Sr Golang Developer  Cupertino, CA (Onsite)-Job Description</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Venkat G &lt;venkat.g@stiorg.com&gt;</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>+1 (740) 3273431, +1 (609) 9983429</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>RE: Sr. Java Lead Consultant available to take new project and open
+ to relocate.</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>"Ishika, Thothit LLC" &lt;ishika@thothit.net&gt;</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>352-614-4461</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>General Database Admin(this is for a DBA not developer)||  Alpharetta, GA(need local with DL)</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>"Riya Kori, Gtech LLC" &lt;rkori@greattechglobal.com&gt;</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>469-527-2150</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>AWS JAVA Engineer || Onsite in Seattle WA || No H1b || Rate is $50 || Ned Aws Active Certification</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>"Shanu, Parmesoft" &lt;shanu.f@parmesoft.com&gt;</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>972-402-5580, 289-652-1056</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Immediate Hire -Oracle EBS PLSQL Developer-Philadelphia, PA(Hybrid)- 12+ plus years of experience</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>"vaibhav kumar, VBeyond Corp" &lt;vaibhavk@vbeyond.com&gt;</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>+1-9086334110</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Sr. Oracle PL-SQL Developer in Chicago, IL (Onsite)</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Murthy Medisetti &lt;murthy@pristineresource.com&gt;</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>860-515-8853, 204565678100</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Techno-Functional Architect (Oracle Revenue Management Cloud
+ Services)</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>"ayush, istaff" &lt;ayush@istaffx.com&gt;</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>575-236-4255</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Java Developer Hybrid role in TX with Selenium Experience Need locals Only in Austin , TX   No h1B</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with Java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>"Suman Bala, HMG America" &lt;sbala@hmgamerica.com&gt;</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>7327905647, 7327905001</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>(Onsite)URGENT REQUIREMENT- SQL Server DBA in Plano TX- onsite</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>(505) 2125488, 467914261938, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Re: Need Power BI with Java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Re: Need Power BI with Java(Must) and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>&lt;prince.sharma@applabsystems.com&gt;</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>2463466860, 2421177820, 609-766-0112</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Oracle Integration Cloud (OIC) || Atlanta, GA; Frisco, TX; Bellevue, WA (Onsite)</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>Ajay Immadisetty &lt;ajay.immadisetty@sitacorp.com&gt;</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>+1 732 9067806</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Oracle HCM Technical Lead/Manager</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>(505) 2125488, 42-9833-474986, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>"Vikas Chaudhary, DMS VISIONS INC" &lt;vikas@dmsvisions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>972-645-0989</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Urgent Hiring || Java Developer || Columbus OH || Hybrid || USC or GC Only || 06 Months C2H || 2nd Round IN person || Local candidates Only Interview</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Vijay &lt;vijay@jnjsolutions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>(505) 2125488, (916) 8581390</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Re: Nee Power BI with java and security for remote</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>"Srikanth, iTech US" &lt;srikanth.v@itechus.net&gt;</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>802 798 8941</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Oracle PL | SQL Developer with Informatica CDI &amp;amp; IICS Exp - Maricopa, AZ(Onsite) - MST | PST Candidates</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>"Gangadar Reddy, Centraprise" &lt;edula.gangadar@centraprise.com&gt;</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>469-639-0369</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Hiring for Java  Engineer II - New York, NY - Day 1 Onsite - AMEX-cognizant</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>"Narsimha Kathi, iTech US" &lt;narsimha.k@itechus.net&gt;</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>802-383-1500, 802-735-0270</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Urgent Requirement for Oracle PLSQL Developer - Phoenix, AZ-Maricopa, AZ - Hybrid Locals or Nearby</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Vishwas Vishwas &lt;vishwasvishwas622@gmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>+1 9105576339</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Re: Sr Golang Developers || Rosemont, IL/Onsite)</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>Faisal Siddiqui &lt;thereisnodifferncebet123@gmail.com&gt;</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>+1 9105576339</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Re: Fwd: Full Stack Java AWS Developer || Seattle, WA (To go onsite 5
+ days a week)</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>"Rajeev, Tek InspirationsLLC" &lt;rajeev.kharwar@tekinspirations.com&gt;</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>7525894499, 469-393-0216</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>AWS PYTHON GOLANG DEVELOPER</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>"Yashwant Singh, DMS Visions Inc" &lt;yashwant@dmsvisions.com&gt;</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>972-645-5050</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>2024-09-30</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Java Developer with CMS and Retail  (Hybrid) Columbus, OH || Locals only || USC &amp;amp; GC only</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>